<commit_message>
remove spaces in headings, uniform "translation" heading
</commit_message>
<xml_diff>
--- a/titlePilotStudy/data/POL.xlsx
+++ b/titlePilotStudy/data/POL.xlsx
@@ -1311,9 +1311,6 @@
   </si>
   <si>
     <t>Which Way? A Contemporary Novel</t>
-  </si>
-  <si>
-    <t>Title - very rough translation</t>
   </si>
   <si>
     <t>In the Petty Bourgeoisies' Nest. A Novel</t>
@@ -1814,6 +1811,9 @@
   </si>
   <si>
     <t>romansik</t>
+  </si>
+  <si>
+    <t>translation</t>
   </si>
 </sst>
 </file>
@@ -2080,13 +2080,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2370,10 +2370,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <selection pane="bottomLeft" activeCell="BZ2" sqref="BZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2496,58 +2496,58 @@
         <v>16</v>
       </c>
       <c r="Y1" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="Z1" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC1" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="AF1" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AG1" s="26" t="s">
         <v>444</v>
       </c>
-      <c r="AB1" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>448</v>
-      </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
         <v>458</v>
       </c>
-      <c r="AE1" s="26" t="s">
-        <v>449</v>
-      </c>
-      <c r="AF1" s="26" t="s">
+      <c r="AK1" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="AL1" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="AG1" s="26" t="s">
+      <c r="AM1" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="AH1" s="26" t="s">
-        <v>450</v>
-      </c>
-      <c r="AI1" s="26" t="s">
-        <v>451</v>
-      </c>
-      <c r="AJ1" s="26" t="s">
+      <c r="AN1" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="AO1" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="AP1" s="26" t="s">
         <v>459</v>
-      </c>
-      <c r="AK1" s="26" t="s">
-        <v>452</v>
-      </c>
-      <c r="AL1" s="26" t="s">
-        <v>443</v>
-      </c>
-      <c r="AM1" s="26" t="s">
-        <v>446</v>
-      </c>
-      <c r="AN1" s="26" t="s">
-        <v>453</v>
-      </c>
-      <c r="AO1" s="26" t="s">
-        <v>454</v>
-      </c>
-      <c r="AP1" s="26" t="s">
-        <v>460</v>
       </c>
       <c r="AQ1" s="14" t="s">
         <v>17</v>
@@ -2562,28 +2562,28 @@
         <v>20</v>
       </c>
       <c r="AU1" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="AV1" s="26" t="s">
         <v>434</v>
       </c>
-      <c r="AV1" s="26" t="s">
+      <c r="AW1" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="AW1" s="26" t="s">
+      <c r="AX1" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="AX1" s="26" t="s">
-        <v>437</v>
-      </c>
       <c r="AY1" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="AZ1" s="26" t="s">
         <v>514</v>
       </c>
-      <c r="AZ1" s="26" t="s">
+      <c r="BA1" s="26" t="s">
         <v>515</v>
       </c>
-      <c r="BA1" s="26" t="s">
+      <c r="BB1" s="26" t="s">
         <v>516</v>
-      </c>
-      <c r="BB1" s="26" t="s">
-        <v>517</v>
       </c>
       <c r="BC1" s="14" t="s">
         <v>21</v>
@@ -2622,16 +2622,16 @@
         <v>33</v>
       </c>
       <c r="BO1" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BP1" s="26" t="s">
         <v>461</v>
       </c>
-      <c r="BP1" s="26" t="s">
+      <c r="BQ1" s="26" t="s">
         <v>462</v>
       </c>
-      <c r="BQ1" s="26" t="s">
+      <c r="BR1" s="26" t="s">
         <v>463</v>
-      </c>
-      <c r="BR1" s="26" t="s">
-        <v>464</v>
       </c>
       <c r="BS1" s="14" t="s">
         <v>34</v>
@@ -2646,16 +2646,16 @@
         <v>37</v>
       </c>
       <c r="BW1" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="BX1" s="26" t="s">
         <v>537</v>
-      </c>
-      <c r="BX1" s="26" t="s">
-        <v>538</v>
       </c>
       <c r="BY1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="BZ1" s="28" t="s">
-        <v>419</v>
+      <c r="BZ1" s="32" t="s">
+        <v>563</v>
       </c>
       <c r="CA1" s="16"/>
       <c r="CB1" s="16"/>
@@ -4155,7 +4155,7 @@
         <v>86</v>
       </c>
       <c r="BZ7" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="CA7" s="23"/>
       <c r="CB7" s="23"/>
@@ -4191,7 +4191,7 @@
       <c r="F8" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="28" t="s">
         <v>89</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -4404,8 +4404,8 @@
       <c r="BY8" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="BZ8" s="30" t="s">
-        <v>421</v>
+      <c r="BZ8" s="29" t="s">
+        <v>420</v>
       </c>
       <c r="CA8" s="23"/>
       <c r="CB8" s="23"/>
@@ -4655,7 +4655,7 @@
         <v>96</v>
       </c>
       <c r="BZ9" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="CA9" s="23"/>
       <c r="CB9" s="23"/>
@@ -4905,7 +4905,7 @@
         <v>99</v>
       </c>
       <c r="BZ10" s="22" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="CA10" s="23"/>
       <c r="CB10" s="23"/>
@@ -5155,7 +5155,7 @@
         <v>104</v>
       </c>
       <c r="BZ11" s="22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="CA11" s="23"/>
       <c r="CB11" s="23"/>
@@ -5345,7 +5345,7 @@
         <v>46</v>
       </c>
       <c r="BF12" s="21" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="BG12" s="21" t="s">
         <v>25</v>
@@ -5404,8 +5404,8 @@
       <c r="BY12" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="BZ12" s="30" t="s">
-        <v>425</v>
+      <c r="BZ12" s="29" t="s">
+        <v>424</v>
       </c>
       <c r="CA12" s="23"/>
       <c r="CB12" s="23"/>
@@ -5655,7 +5655,7 @@
         <v>114</v>
       </c>
       <c r="BZ13" s="22" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="CA13" s="23"/>
       <c r="CB13" s="23"/>
@@ -5707,7 +5707,7 @@
         <v>46</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>46</v>
@@ -5904,8 +5904,8 @@
       <c r="BY14" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="BZ14" s="30" t="s">
-        <v>428</v>
+      <c r="BZ14" s="29" t="s">
+        <v>427</v>
       </c>
       <c r="CA14" s="23"/>
       <c r="CB14" s="23"/>
@@ -6154,8 +6154,8 @@
       <c r="BY15" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="BZ15" s="30" t="s">
-        <v>429</v>
+      <c r="BZ15" s="29" t="s">
+        <v>428</v>
       </c>
       <c r="CA15" s="23"/>
       <c r="CB15" s="23"/>
@@ -6404,8 +6404,8 @@
       <c r="BY16" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="BZ16" s="30" t="s">
-        <v>430</v>
+      <c r="BZ16" s="29" t="s">
+        <v>429</v>
       </c>
       <c r="CA16" s="23"/>
       <c r="CB16" s="23"/>
@@ -6484,7 +6484,7 @@
         <v>25</v>
       </c>
       <c r="U17" s="21" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="V17" s="21" t="s">
         <v>25</v>
@@ -6553,7 +6553,7 @@
         <v>80</v>
       </c>
       <c r="AR17" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AS17" s="21" t="s">
         <v>25</v>
@@ -6565,7 +6565,7 @@
         <v>80</v>
       </c>
       <c r="AV17" s="21" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AW17" s="21" t="s">
         <v>25</v>
@@ -6595,7 +6595,7 @@
         <v>46</v>
       </c>
       <c r="BF17" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="BG17" s="21" t="s">
         <v>25</v>
@@ -6652,10 +6652,10 @@
         <v>25</v>
       </c>
       <c r="BY17" s="21" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="BZ17" s="22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="CA17" s="23"/>
       <c r="CB17" s="23"/>
@@ -6752,7 +6752,7 @@
         <v>25</v>
       </c>
       <c r="AA18" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AB18" s="21" t="s">
         <v>25</v>
@@ -6770,7 +6770,7 @@
         <v>25</v>
       </c>
       <c r="AG18" s="21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AH18" s="21" t="s">
         <v>25</v>
@@ -6788,7 +6788,7 @@
         <v>25</v>
       </c>
       <c r="AM18" s="21" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AN18" s="21" t="s">
         <v>25</v>
@@ -6845,7 +6845,7 @@
         <v>46</v>
       </c>
       <c r="BF18" s="21" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="BG18" s="21" t="s">
         <v>25</v>
@@ -6904,8 +6904,8 @@
       <c r="BY18" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="BZ18" s="30" t="s">
-        <v>466</v>
+      <c r="BZ18" s="29" t="s">
+        <v>465</v>
       </c>
       <c r="CA18" s="23"/>
       <c r="CB18" s="23"/>
@@ -6999,10 +6999,10 @@
         <v>46</v>
       </c>
       <c r="Z19" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="AA19" s="21" t="s">
         <v>467</v>
-      </c>
-      <c r="AA19" s="21" t="s">
-        <v>468</v>
       </c>
       <c r="AB19" s="21" t="s">
         <v>25</v>
@@ -7053,7 +7053,7 @@
         <v>129</v>
       </c>
       <c r="AR19" s="21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AS19" s="21" t="s">
         <v>25</v>
@@ -7095,7 +7095,7 @@
         <v>46</v>
       </c>
       <c r="BF19" s="21" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="BG19" s="21" t="s">
         <v>25</v>
@@ -7154,8 +7154,8 @@
       <c r="BY19" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="BZ19" s="30" t="s">
-        <v>470</v>
+      <c r="BZ19" s="29" t="s">
+        <v>469</v>
       </c>
       <c r="CA19" s="23"/>
       <c r="CB19" s="23"/>
@@ -7404,8 +7404,8 @@
       <c r="BY20" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="BZ20" s="30" t="s">
-        <v>471</v>
+      <c r="BZ20" s="29" t="s">
+        <v>470</v>
       </c>
       <c r="CA20" s="23"/>
       <c r="CB20" s="23"/>
@@ -7553,7 +7553,7 @@
         <v>80</v>
       </c>
       <c r="AR21" s="21" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AS21" s="21" t="s">
         <v>25</v>
@@ -7595,7 +7595,7 @@
         <v>46</v>
       </c>
       <c r="BF21" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="BG21" s="21" t="s">
         <v>25</v>
@@ -7654,8 +7654,8 @@
       <c r="BY21" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="BZ21" s="30" t="s">
-        <v>474</v>
+      <c r="BZ21" s="29" t="s">
+        <v>473</v>
       </c>
       <c r="CA21" s="23"/>
       <c r="CB21" s="23"/>
@@ -7815,7 +7815,7 @@
         <v>129</v>
       </c>
       <c r="AV22" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AW22" s="21" t="s">
         <v>25</v>
@@ -7904,8 +7904,8 @@
       <c r="BY22" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="BZ22" s="30" t="s">
-        <v>476</v>
+      <c r="BZ22" s="29" t="s">
+        <v>475</v>
       </c>
       <c r="CA22" s="23"/>
       <c r="CB22" s="23"/>
@@ -8155,7 +8155,7 @@
         <v>25</v>
       </c>
       <c r="BZ23" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="CA23" s="23"/>
       <c r="CB23" s="23"/>
@@ -8405,7 +8405,7 @@
         <v>154</v>
       </c>
       <c r="BZ24" s="22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CA24" s="23"/>
       <c r="CB24" s="23"/>
@@ -8654,8 +8654,8 @@
       <c r="BY25" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="BZ25" s="30" t="s">
-        <v>479</v>
+      <c r="BZ25" s="29" t="s">
+        <v>478</v>
       </c>
       <c r="CA25" s="23"/>
       <c r="CB25" s="23"/>
@@ -8904,8 +8904,8 @@
       <c r="BY26" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="BZ26" s="30" t="s">
-        <v>480</v>
+      <c r="BZ26" s="29" t="s">
+        <v>479</v>
       </c>
       <c r="CA26" s="23"/>
       <c r="CB26" s="23"/>
@@ -9155,7 +9155,7 @@
         <v>166</v>
       </c>
       <c r="BZ27" s="22" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="CA27" s="23"/>
       <c r="CB27" s="23"/>
@@ -9252,7 +9252,7 @@
         <v>25</v>
       </c>
       <c r="AA28" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AB28" s="21" t="s">
         <v>25</v>
@@ -9404,8 +9404,8 @@
       <c r="BY28" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="BZ28" s="30" t="s">
-        <v>483</v>
+      <c r="BZ28" s="29" t="s">
+        <v>482</v>
       </c>
       <c r="CA28" s="23"/>
       <c r="CB28" s="23"/>
@@ -9654,8 +9654,8 @@
       <c r="BY29" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="BZ29" s="30" t="s">
-        <v>484</v>
+      <c r="BZ29" s="29" t="s">
+        <v>483</v>
       </c>
       <c r="CA29" s="23"/>
       <c r="CB29" s="23"/>
@@ -9904,8 +9904,8 @@
       <c r="BY30" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="BZ30" s="30" t="s">
-        <v>485</v>
+      <c r="BZ30" s="29" t="s">
+        <v>484</v>
       </c>
       <c r="CA30" s="23"/>
       <c r="CB30" s="23"/>
@@ -10154,8 +10154,8 @@
       <c r="BY31" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="BZ31" s="30" t="s">
-        <v>486</v>
+      <c r="BZ31" s="29" t="s">
+        <v>485</v>
       </c>
       <c r="CA31" s="23"/>
       <c r="CB31" s="23"/>
@@ -10404,8 +10404,8 @@
       <c r="BY32" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="BZ32" s="30" t="s">
-        <v>487</v>
+      <c r="BZ32" s="29" t="s">
+        <v>486</v>
       </c>
       <c r="CA32" s="23"/>
       <c r="CB32" s="23"/>
@@ -10502,7 +10502,7 @@
         <v>25</v>
       </c>
       <c r="AA33" s="21" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AB33" s="21" t="s">
         <v>25</v>
@@ -10654,8 +10654,8 @@
       <c r="BY33" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="BZ33" s="30" t="s">
-        <v>488</v>
+      <c r="BZ33" s="29" t="s">
+        <v>487</v>
       </c>
       <c r="CA33" s="23"/>
       <c r="CB33" s="23"/>
@@ -10815,7 +10815,7 @@
         <v>80</v>
       </c>
       <c r="AV34" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AW34" s="21" t="s">
         <v>25</v>
@@ -10904,8 +10904,8 @@
       <c r="BY34" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="BZ34" s="30" t="s">
-        <v>490</v>
+      <c r="BZ34" s="29" t="s">
+        <v>489</v>
       </c>
       <c r="CA34" s="23"/>
       <c r="CB34" s="23"/>
@@ -11095,7 +11095,7 @@
         <v>46</v>
       </c>
       <c r="BF35" s="21" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="BG35" s="21" t="s">
         <v>25</v>
@@ -11154,8 +11154,8 @@
       <c r="BY35" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="BZ35" s="30" t="s">
-        <v>491</v>
+      <c r="BZ35" s="29" t="s">
+        <v>490</v>
       </c>
       <c r="CA35" s="23"/>
       <c r="CB35" s="23"/>
@@ -11404,8 +11404,8 @@
       <c r="BY36" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="BZ36" s="30" t="s">
-        <v>492</v>
+      <c r="BZ36" s="29" t="s">
+        <v>491</v>
       </c>
       <c r="CA36" s="23"/>
       <c r="CB36" s="23"/>
@@ -11655,7 +11655,7 @@
         <v>203</v>
       </c>
       <c r="BZ37" s="22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="CA37" s="23"/>
       <c r="CB37" s="23"/>
@@ -11691,8 +11691,8 @@
       <c r="F38" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="29" t="s">
-        <v>496</v>
+      <c r="G38" s="28" t="s">
+        <v>495</v>
       </c>
       <c r="H38" s="18" t="s">
         <v>197</v>
@@ -11752,7 +11752,7 @@
         <v>25</v>
       </c>
       <c r="AA38" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AB38" s="21" t="s">
         <v>25</v>
@@ -11803,7 +11803,7 @@
         <v>129</v>
       </c>
       <c r="AR38" s="21" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AS38" s="21" t="s">
         <v>25</v>
@@ -11815,7 +11815,7 @@
         <v>129</v>
       </c>
       <c r="AV38" s="21" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AW38" s="21" t="s">
         <v>25</v>
@@ -11904,8 +11904,8 @@
       <c r="BY38" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="BZ38" s="30" t="s">
-        <v>494</v>
+      <c r="BZ38" s="29" t="s">
+        <v>493</v>
       </c>
       <c r="CA38" s="23"/>
       <c r="CB38" s="23"/>
@@ -12154,8 +12154,8 @@
       <c r="BY39" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="BZ39" s="30" t="s">
-        <v>499</v>
+      <c r="BZ39" s="29" t="s">
+        <v>498</v>
       </c>
       <c r="CA39" s="23"/>
       <c r="CB39" s="23"/>
@@ -12249,10 +12249,10 @@
         <v>46</v>
       </c>
       <c r="Z40" s="21" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AA40" s="21" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AB40" s="21" t="s">
         <v>25</v>
@@ -12404,8 +12404,8 @@
       <c r="BY40" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="BZ40" s="30" t="s">
-        <v>501</v>
+      <c r="BZ40" s="29" t="s">
+        <v>500</v>
       </c>
       <c r="CA40" s="23"/>
       <c r="CB40" s="23"/>
@@ -12595,7 +12595,7 @@
         <v>46</v>
       </c>
       <c r="BF41" s="21" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BG41" s="21" t="s">
         <v>25</v>
@@ -12654,8 +12654,8 @@
       <c r="BY41" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="BZ41" s="30" t="s">
-        <v>502</v>
+      <c r="BZ41" s="29" t="s">
+        <v>501</v>
       </c>
       <c r="CA41" s="23"/>
       <c r="CB41" s="23"/>
@@ -12803,7 +12803,7 @@
         <v>129</v>
       </c>
       <c r="AR42" s="21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AS42" s="21" t="s">
         <v>25</v>
@@ -12815,7 +12815,7 @@
         <v>80</v>
       </c>
       <c r="AV42" s="21" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AW42" s="21" t="s">
         <v>25</v>
@@ -12904,8 +12904,8 @@
       <c r="BY42" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="BZ42" s="30" t="s">
-        <v>505</v>
+      <c r="BZ42" s="29" t="s">
+        <v>504</v>
       </c>
       <c r="CA42" s="23"/>
       <c r="CB42" s="23"/>
@@ -13155,7 +13155,7 @@
         <v>227</v>
       </c>
       <c r="BZ43" s="22" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="CA43" s="23"/>
       <c r="CB43" s="23"/>
@@ -13405,7 +13405,7 @@
         <v>232</v>
       </c>
       <c r="BZ44" s="22" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="CA44" s="23"/>
       <c r="CB44" s="23"/>
@@ -13441,7 +13441,7 @@
       <c r="F45" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="30" t="s">
         <v>235</v>
       </c>
       <c r="H45" s="18" t="s">
@@ -13499,10 +13499,10 @@
         <v>46</v>
       </c>
       <c r="Z45" s="21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AA45" s="21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AB45" s="21" t="s">
         <v>46</v>
@@ -13565,7 +13565,7 @@
         <v>80</v>
       </c>
       <c r="AV45" s="21" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="AW45" s="21" t="s">
         <v>25</v>
@@ -13654,8 +13654,8 @@
       <c r="BY45" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="BZ45" s="32" t="s">
-        <v>509</v>
+      <c r="BZ45" s="31" t="s">
+        <v>508</v>
       </c>
       <c r="CA45" s="23"/>
       <c r="CB45" s="23"/>
@@ -13803,7 +13803,7 @@
         <v>129</v>
       </c>
       <c r="AR46" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AS46" s="21" t="s">
         <v>25</v>
@@ -13815,7 +13815,7 @@
         <v>80</v>
       </c>
       <c r="AV46" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AW46" s="21" t="s">
         <v>25</v>
@@ -13904,8 +13904,8 @@
       <c r="BY46" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="BZ46" s="32" t="s">
-        <v>511</v>
+      <c r="BZ46" s="31" t="s">
+        <v>510</v>
       </c>
       <c r="CA46" s="23"/>
       <c r="CB46" s="23"/>
@@ -13984,7 +13984,7 @@
         <v>25</v>
       </c>
       <c r="U47" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="V47" s="21" t="s">
         <v>46</v>
@@ -14154,8 +14154,8 @@
       <c r="BY47" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="BZ47" s="32" t="s">
-        <v>519</v>
+      <c r="BZ47" s="31" t="s">
+        <v>518</v>
       </c>
       <c r="CA47" s="23"/>
       <c r="CB47" s="23"/>
@@ -14904,7 +14904,7 @@
       <c r="BY50" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="BZ50" s="32" t="s">
+      <c r="BZ50" s="31" t="s">
         <v>258</v>
       </c>
       <c r="CA50" s="23"/>
@@ -14984,7 +14984,7 @@
         <v>25</v>
       </c>
       <c r="U51" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="V51" s="21" t="s">
         <v>25</v>
@@ -15154,8 +15154,8 @@
       <c r="BY51" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="BZ51" s="32" t="s">
-        <v>520</v>
+      <c r="BZ51" s="31" t="s">
+        <v>519</v>
       </c>
       <c r="CA51" s="23"/>
       <c r="CB51" s="23"/>
@@ -15484,7 +15484,7 @@
         <v>25</v>
       </c>
       <c r="U53" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="V53" s="21" t="s">
         <v>25</v>
@@ -15565,7 +15565,7 @@
         <v>80</v>
       </c>
       <c r="AV53" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AW53" s="21" t="s">
         <v>25</v>
@@ -15654,8 +15654,8 @@
       <c r="BY53" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="BZ53" s="32" t="s">
-        <v>522</v>
+      <c r="BZ53" s="31" t="s">
+        <v>521</v>
       </c>
       <c r="CA53" s="23"/>
       <c r="CB53" s="23"/>
@@ -15904,8 +15904,8 @@
       <c r="BY54" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="BZ54" s="32" t="s">
-        <v>523</v>
+      <c r="BZ54" s="31" t="s">
+        <v>522</v>
       </c>
       <c r="CA54" s="23"/>
       <c r="CB54" s="23"/>
@@ -16154,8 +16154,8 @@
       <c r="BY55" s="21" t="s">
         <v>277</v>
       </c>
-      <c r="BZ55" s="32" t="s">
-        <v>530</v>
+      <c r="BZ55" s="31" t="s">
+        <v>529</v>
       </c>
       <c r="CA55" s="23"/>
       <c r="CB55" s="23"/>
@@ -16315,10 +16315,10 @@
         <v>129</v>
       </c>
       <c r="AV56" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="AW56" s="21" t="s">
         <v>531</v>
-      </c>
-      <c r="AW56" s="21" t="s">
-        <v>532</v>
       </c>
       <c r="AX56" s="21" t="s">
         <v>25</v>
@@ -16405,7 +16405,7 @@
         <v>280</v>
       </c>
       <c r="BZ56" s="22" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="CA56" s="23"/>
       <c r="CB56" s="23"/>
@@ -16654,8 +16654,8 @@
       <c r="BY57" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="BZ57" s="32" t="s">
-        <v>528</v>
+      <c r="BZ57" s="31" t="s">
+        <v>527</v>
       </c>
       <c r="CA57" s="23"/>
       <c r="CB57" s="23"/>
@@ -16905,7 +16905,7 @@
         <v>287</v>
       </c>
       <c r="BZ58" s="22" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="CA58" s="23"/>
       <c r="CB58" s="23"/>
@@ -17404,8 +17404,8 @@
       <c r="BY60" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="BZ60" s="32" t="s">
-        <v>526</v>
+      <c r="BZ60" s="31" t="s">
+        <v>525</v>
       </c>
       <c r="CA60" s="23"/>
       <c r="CB60" s="23"/>
@@ -17565,7 +17565,7 @@
         <v>80</v>
       </c>
       <c r="AV61" s="21" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AW61" s="21" t="s">
         <v>25</v>
@@ -17654,8 +17654,8 @@
       <c r="BY61" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="BZ61" s="32" t="s">
-        <v>525</v>
+      <c r="BZ61" s="31" t="s">
+        <v>524</v>
       </c>
       <c r="CA61" s="23"/>
       <c r="CB61" s="23"/>
@@ -17904,8 +17904,8 @@
       <c r="BY62" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="BZ62" s="32" t="s">
-        <v>533</v>
+      <c r="BZ62" s="31" t="s">
+        <v>532</v>
       </c>
       <c r="CA62" s="23"/>
       <c r="CB62" s="23"/>
@@ -18065,7 +18065,7 @@
         <v>80</v>
       </c>
       <c r="AV63" s="21" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AW63" s="21" t="s">
         <v>25</v>
@@ -18077,7 +18077,7 @@
         <v>129</v>
       </c>
       <c r="AZ63" s="21" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="BA63" s="21" t="s">
         <v>25</v>
@@ -18154,8 +18154,8 @@
       <c r="BY63" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="BZ63" s="32" t="s">
-        <v>534</v>
+      <c r="BZ63" s="31" t="s">
+        <v>533</v>
       </c>
       <c r="CA63" s="23"/>
       <c r="CB63" s="23"/>
@@ -18234,7 +18234,7 @@
         <v>25</v>
       </c>
       <c r="U64" s="21" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V64" s="21" t="s">
         <v>25</v>
@@ -18404,8 +18404,8 @@
       <c r="BY64" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="BZ64" s="32" t="s">
-        <v>539</v>
+      <c r="BZ64" s="31" t="s">
+        <v>538</v>
       </c>
       <c r="CA64" s="23"/>
       <c r="CB64" s="23"/>
@@ -18654,8 +18654,8 @@
       <c r="BY65" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="BZ65" s="32" t="s">
-        <v>541</v>
+      <c r="BZ65" s="31" t="s">
+        <v>540</v>
       </c>
       <c r="CA65" s="23"/>
       <c r="CB65" s="23"/>
@@ -18803,7 +18803,7 @@
         <v>129</v>
       </c>
       <c r="AR66" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AS66" s="21" t="s">
         <v>25</v>
@@ -18904,8 +18904,8 @@
       <c r="BY66" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="BZ66" s="32" t="s">
-        <v>542</v>
+      <c r="BZ66" s="31" t="s">
+        <v>541</v>
       </c>
       <c r="CA66" s="23"/>
       <c r="CB66" s="23"/>
@@ -19154,8 +19154,8 @@
       <c r="BY67" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="BZ67" s="32" t="s">
-        <v>543</v>
+      <c r="BZ67" s="31" t="s">
+        <v>542</v>
       </c>
       <c r="CA67" s="23"/>
       <c r="CB67" s="23"/>
@@ -19442,7 +19442,7 @@
         <v>54</v>
       </c>
       <c r="G69" s="18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H69" s="18" t="s">
         <v>330</v>
@@ -19457,7 +19457,7 @@
         <v>46</v>
       </c>
       <c r="L69" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="M69" s="21" t="s">
         <v>46</v>
@@ -19484,7 +19484,7 @@
         <v>25</v>
       </c>
       <c r="U69" s="21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V69" s="21" t="s">
         <v>46</v>
@@ -19652,10 +19652,10 @@
         <v>25</v>
       </c>
       <c r="BY69" s="21" t="s">
+        <v>545</v>
+      </c>
+      <c r="BZ69" s="31" t="s">
         <v>546</v>
-      </c>
-      <c r="BZ69" s="32" t="s">
-        <v>547</v>
       </c>
       <c r="CA69" s="23"/>
       <c r="CB69" s="23"/>
@@ -19904,8 +19904,8 @@
       <c r="BY70" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="BZ70" s="32" t="s">
-        <v>548</v>
+      <c r="BZ70" s="31" t="s">
+        <v>547</v>
       </c>
       <c r="CA70" s="23"/>
       <c r="CB70" s="23"/>
@@ -20154,8 +20154,8 @@
       <c r="BY71" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="BZ71" s="32" t="s">
-        <v>549</v>
+      <c r="BZ71" s="31" t="s">
+        <v>548</v>
       </c>
       <c r="CA71" s="23"/>
       <c r="CB71" s="23"/>
@@ -20405,7 +20405,7 @@
         <v>342</v>
       </c>
       <c r="BZ72" s="22" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="CA72" s="23"/>
       <c r="CB72" s="23"/>
@@ -20654,8 +20654,8 @@
       <c r="BY73" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="BZ73" s="32" t="s">
-        <v>551</v>
+      <c r="BZ73" s="31" t="s">
+        <v>550</v>
       </c>
       <c r="CA73" s="23"/>
       <c r="CB73" s="23"/>
@@ -20904,8 +20904,8 @@
       <c r="BY74" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="BZ74" s="32" t="s">
-        <v>552</v>
+      <c r="BZ74" s="31" t="s">
+        <v>551</v>
       </c>
       <c r="CA74" s="23"/>
       <c r="CB74" s="23"/>
@@ -22442,7 +22442,7 @@
         <v>159</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H81" s="18" t="s">
         <v>379</v>
@@ -22553,7 +22553,7 @@
         <v>129</v>
       </c>
       <c r="AR81" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AS81" s="21" t="s">
         <v>25</v>
@@ -22565,7 +22565,7 @@
         <v>80</v>
       </c>
       <c r="AV81" s="21" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AW81" s="21" t="s">
         <v>25</v>
@@ -22654,8 +22654,8 @@
       <c r="BY81" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="BZ81" s="32" t="s">
-        <v>556</v>
+      <c r="BZ81" s="31" t="s">
+        <v>555</v>
       </c>
       <c r="CA81" s="23"/>
       <c r="CB81" s="23"/>
@@ -22803,7 +22803,7 @@
         <v>80</v>
       </c>
       <c r="AR82" s="21" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AS82" s="21" t="s">
         <v>25</v>
@@ -22904,8 +22904,8 @@
       <c r="BY82" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="BZ82" s="32" t="s">
-        <v>557</v>
+      <c r="BZ82" s="31" t="s">
+        <v>556</v>
       </c>
       <c r="CA82" s="23"/>
       <c r="CB82" s="23"/>
@@ -23065,7 +23065,7 @@
         <v>80</v>
       </c>
       <c r="AV83" s="21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AW83" s="21" t="s">
         <v>25</v>
@@ -23154,8 +23154,8 @@
       <c r="BY83" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="BZ83" s="32" t="s">
-        <v>558</v>
+      <c r="BZ83" s="31" t="s">
+        <v>557</v>
       </c>
       <c r="CA83" s="23"/>
       <c r="CB83" s="23"/>
@@ -23404,8 +23404,8 @@
       <c r="BY84" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="BZ84" s="32" t="s">
-        <v>560</v>
+      <c r="BZ84" s="31" t="s">
+        <v>559</v>
       </c>
       <c r="CA84" s="23"/>
       <c r="CB84" s="23"/>

</xml_diff>